<commit_message>
Finish TODC age, grade ru-runs
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/gea_sum-raw-ss-lookup-tabbed-grade.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/gea_sum-raw-ss-lookup-tabbed-grade.xlsx
@@ -413,7 +413,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5">
@@ -421,7 +421,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
@@ -429,7 +429,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7">
@@ -437,7 +437,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8">
@@ -445,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9">
@@ -453,7 +453,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
@@ -461,7 +461,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
@@ -469,7 +469,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12">
@@ -477,7 +477,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -485,7 +485,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14">
@@ -493,7 +493,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15">
@@ -501,7 +501,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16">
@@ -509,7 +509,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17">
@@ -517,7 +517,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18">
@@ -525,7 +525,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19">
@@ -533,7 +533,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20">
@@ -541,7 +541,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21">
@@ -549,7 +549,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22">
@@ -557,7 +557,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23">
@@ -565,7 +565,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24">
@@ -814,7 +814,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11">
@@ -822,7 +822,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12">
@@ -830,7 +830,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13">
@@ -982,7 +982,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32">
@@ -990,7 +990,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33">
@@ -998,7 +998,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34">
@@ -1006,7 +1006,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35">
@@ -1014,7 +1014,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36">
@@ -1022,7 +1022,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37">
@@ -1135,7 +1135,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
@@ -1143,7 +1143,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
@@ -1151,7 +1151,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9">
@@ -1159,7 +1159,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10">
@@ -1215,7 +1215,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17">
@@ -1223,7 +1223,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18">
@@ -1335,7 +1335,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32">
@@ -1343,7 +1343,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33">
@@ -1359,7 +1359,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35">
@@ -1367,7 +1367,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36">
@@ -1375,7 +1375,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37">
@@ -1383,7 +1383,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38">
@@ -1472,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
@@ -1480,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
@@ -1488,7 +1488,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
@@ -1496,7 +1496,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
@@ -1504,7 +1504,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
@@ -1512,7 +1512,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
@@ -1528,7 +1528,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12">
@@ -1536,7 +1536,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13">
@@ -1544,7 +1544,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14">
@@ -1552,7 +1552,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15">
@@ -1560,7 +1560,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
@@ -1624,7 +1624,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24">
@@ -1632,7 +1632,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25">
@@ -1640,7 +1640,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26">
@@ -1648,7 +1648,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27">
@@ -1656,7 +1656,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
@@ -1664,7 +1664,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29">
@@ -1704,7 +1704,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34">
@@ -1712,7 +1712,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35">
@@ -1720,7 +1720,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36">
@@ -1728,7 +1728,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37">
@@ -1736,7 +1736,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38">
@@ -1809,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
@@ -1817,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
@@ -1825,7 +1825,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
@@ -1833,7 +1833,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
@@ -1841,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
@@ -1849,7 +1849,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8">
@@ -1857,7 +1857,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9">
@@ -1865,7 +1865,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
@@ -1873,7 +1873,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
@@ -1881,7 +1881,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12">
@@ -1889,7 +1889,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13">
@@ -1897,7 +1897,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14">
@@ -1905,7 +1905,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
@@ -1937,7 +1937,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19">
@@ -1945,7 +1945,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20">
@@ -1953,7 +1953,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21">
@@ -2041,7 +2041,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32">
@@ -2065,7 +2065,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35">
@@ -2073,7 +2073,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36">
@@ -2081,7 +2081,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37">
@@ -2089,7 +2089,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38">
@@ -2097,7 +2097,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39">
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -2170,7 +2170,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
@@ -2178,7 +2178,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -2186,7 +2186,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
@@ -2194,7 +2194,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7">
@@ -2202,7 +2202,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8">
@@ -2210,7 +2210,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
@@ -2218,7 +2218,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10">
@@ -2226,7 +2226,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
@@ -2234,7 +2234,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12">
@@ -2242,7 +2242,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13">
@@ -2250,7 +2250,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14">
@@ -2258,7 +2258,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15">
@@ -2266,7 +2266,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16">
@@ -2274,7 +2274,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
@@ -2282,7 +2282,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
@@ -2290,7 +2290,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
@@ -2298,7 +2298,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20">
@@ -2426,7 +2426,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36">
@@ -2434,7 +2434,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37">
@@ -2442,7 +2442,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38">
@@ -2450,7 +2450,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39">
@@ -2515,7 +2515,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
@@ -2523,7 +2523,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
@@ -2531,7 +2531,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5">
@@ -2539,7 +2539,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -2547,7 +2547,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
@@ -2555,7 +2555,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
@@ -2563,7 +2563,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9">
@@ -2571,7 +2571,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
@@ -2579,7 +2579,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11">
@@ -2587,7 +2587,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
@@ -2595,7 +2595,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
@@ -2603,7 +2603,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14">
@@ -2611,7 +2611,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15">
@@ -2619,7 +2619,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -2627,7 +2627,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17">
@@ -2635,7 +2635,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18">
@@ -2643,7 +2643,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
@@ -2651,7 +2651,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20">
@@ -2715,7 +2715,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28">
@@ -2723,7 +2723,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29">
@@ -2763,7 +2763,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34">
@@ -2779,7 +2779,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36">
@@ -2787,7 +2787,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37">
@@ -2795,7 +2795,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38">
@@ -2803,7 +2803,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39">
@@ -2811,7 +2811,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40">
@@ -2868,7 +2868,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
@@ -2876,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
@@ -2884,7 +2884,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
@@ -2892,7 +2892,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
@@ -2900,7 +2900,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7">
@@ -2908,7 +2908,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8">
@@ -2916,7 +2916,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9">
@@ -2924,7 +2924,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
@@ -2932,7 +2932,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11">
@@ -2940,7 +2940,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12">
@@ -2948,7 +2948,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13">
@@ -2956,7 +2956,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
@@ -2964,7 +2964,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15">
@@ -2972,7 +2972,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
@@ -2980,7 +2980,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
@@ -2988,7 +2988,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
@@ -2996,7 +2996,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
@@ -3004,7 +3004,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20">
@@ -3012,7 +3012,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21">
@@ -3076,7 +3076,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29">
@@ -3108,7 +3108,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33">
@@ -3116,7 +3116,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34">
@@ -3132,7 +3132,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36">
@@ -3140,7 +3140,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37">
@@ -3148,7 +3148,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38">
@@ -3156,7 +3156,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39">
@@ -3164,7 +3164,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40">
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
@@ -3229,7 +3229,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -3237,7 +3237,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
@@ -3245,7 +3245,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
@@ -3253,7 +3253,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -3261,7 +3261,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
@@ -3269,7 +3269,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
@@ -3277,7 +3277,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10">
@@ -3285,7 +3285,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11">
@@ -3293,7 +3293,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
@@ -3309,7 +3309,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14">
@@ -3317,7 +3317,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
@@ -3325,7 +3325,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
@@ -3333,7 +3333,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
@@ -3341,7 +3341,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -3349,7 +3349,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19">
@@ -3357,7 +3357,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
@@ -3365,7 +3365,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
@@ -3373,7 +3373,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22">
@@ -3453,7 +3453,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32">
@@ -3461,7 +3461,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33">
@@ -3493,7 +3493,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37">
@@ -3501,7 +3501,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38">
@@ -3509,7 +3509,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39">
@@ -3517,7 +3517,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40">
@@ -3574,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
@@ -3582,7 +3582,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -3590,7 +3590,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
@@ -3598,7 +3598,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
@@ -3606,7 +3606,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7">
@@ -3614,7 +3614,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
@@ -3622,7 +3622,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9">
@@ -3630,7 +3630,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10">
@@ -3638,7 +3638,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
@@ -3646,7 +3646,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12">
@@ -3654,7 +3654,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
@@ -3662,7 +3662,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
@@ -3670,7 +3670,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
@@ -3678,7 +3678,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
@@ -3686,7 +3686,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
@@ -3694,7 +3694,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
@@ -3702,7 +3702,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
@@ -3710,7 +3710,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
@@ -3718,7 +3718,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -3726,7 +3726,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22">
@@ -3734,7 +3734,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23">
@@ -3742,7 +3742,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24">
@@ -3790,7 +3790,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30">
@@ -3798,7 +3798,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31">
@@ -3806,7 +3806,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32">
@@ -3814,7 +3814,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33">
@@ -3830,7 +3830,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35">
@@ -3854,7 +3854,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38">
@@ -3862,7 +3862,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39">
@@ -3870,7 +3870,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40">
@@ -3927,7 +3927,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
@@ -3935,7 +3935,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
@@ -3943,7 +3943,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
@@ -3951,7 +3951,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
@@ -3959,7 +3959,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
@@ -3967,7 +3967,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
@@ -3975,7 +3975,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -3983,7 +3983,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10">
@@ -3991,7 +3991,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11">
@@ -3999,7 +3999,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
@@ -4007,7 +4007,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13">
@@ -4015,7 +4015,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
@@ -4023,7 +4023,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
@@ -4031,7 +4031,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
@@ -4039,7 +4039,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17">
@@ -4047,7 +4047,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -4055,7 +4055,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
@@ -4063,7 +4063,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -4071,7 +4071,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21">
@@ -4079,7 +4079,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22">
@@ -4087,7 +4087,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23">
@@ -4095,7 +4095,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24">
@@ -4103,7 +4103,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25">
@@ -4111,7 +4111,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26">
@@ -4119,7 +4119,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27">
@@ -4135,7 +4135,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29">
@@ -4143,7 +4143,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30">
@@ -4167,7 +4167,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33">
@@ -4175,7 +4175,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34">
@@ -4199,7 +4199,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37">
@@ -4207,7 +4207,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38">
@@ -4215,7 +4215,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39">
@@ -4223,7 +4223,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40">
@@ -4288,7 +4288,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
@@ -4312,7 +4312,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
@@ -4320,7 +4320,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8">
@@ -4328,7 +4328,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9">
@@ -4336,7 +4336,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10">
@@ -4344,7 +4344,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11">
@@ -4352,7 +4352,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12">
@@ -4360,7 +4360,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13">
@@ -4368,7 +4368,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14">
@@ -4376,7 +4376,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15">
@@ -4384,7 +4384,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16">
@@ -4392,7 +4392,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17">
@@ -4400,7 +4400,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18">
@@ -4408,7 +4408,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19">
@@ -4416,7 +4416,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20">
@@ -4424,7 +4424,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21">
@@ -4432,7 +4432,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22">
@@ -4440,7 +4440,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23">
@@ -4448,7 +4448,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24">
@@ -4456,7 +4456,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25">
@@ -4464,7 +4464,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26">
@@ -4472,7 +4472,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27">
@@ -4633,7 +4633,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
@@ -4641,7 +4641,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -4649,7 +4649,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
@@ -4657,7 +4657,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
@@ -4665,7 +4665,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7">
@@ -4673,7 +4673,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
@@ -4681,7 +4681,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -4689,7 +4689,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
@@ -4697,7 +4697,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11">
@@ -4705,7 +4705,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
@@ -4713,7 +4713,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13">
@@ -4721,7 +4721,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
@@ -4729,7 +4729,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -4737,7 +4737,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
@@ -4745,7 +4745,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
@@ -4753,7 +4753,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
@@ -4761,7 +4761,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
@@ -4769,7 +4769,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20">
@@ -4777,7 +4777,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21">
@@ -4785,7 +4785,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22">
@@ -4793,7 +4793,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23">
@@ -4801,7 +4801,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24">
@@ -4809,7 +4809,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25">
@@ -4857,7 +4857,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31">
@@ -4865,7 +4865,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32">
@@ -4881,7 +4881,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34">
@@ -4897,7 +4897,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36">
@@ -4905,7 +4905,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37">
@@ -4913,7 +4913,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38">
@@ -4921,7 +4921,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39">
@@ -4929,7 +4929,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40">
@@ -4986,7 +4986,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -4994,7 +4994,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -5002,7 +5002,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
@@ -5010,7 +5010,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
@@ -5018,7 +5018,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
@@ -5026,7 +5026,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
@@ -5034,7 +5034,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9">
@@ -5042,7 +5042,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
@@ -5050,7 +5050,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -5058,7 +5058,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
@@ -5066,7 +5066,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
@@ -5074,7 +5074,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14">
@@ -5082,7 +5082,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -5090,7 +5090,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
@@ -5098,7 +5098,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
@@ -5106,7 +5106,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18">
@@ -5114,7 +5114,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
@@ -5122,7 +5122,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20">
@@ -5130,7 +5130,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21">
@@ -5138,7 +5138,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22">
@@ -5146,7 +5146,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23">
@@ -5154,7 +5154,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24">
@@ -5162,7 +5162,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25">
@@ -5170,7 +5170,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26">
@@ -5178,7 +5178,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27">
@@ -5186,7 +5186,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28">
@@ -5218,7 +5218,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32">
@@ -5226,7 +5226,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33">
@@ -5234,7 +5234,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34">
@@ -5266,7 +5266,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38">
@@ -5274,7 +5274,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39">
@@ -5282,7 +5282,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40">
@@ -5339,7 +5339,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -5347,7 +5347,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -5355,7 +5355,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
@@ -5363,7 +5363,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6">
@@ -5371,7 +5371,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
@@ -5379,7 +5379,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
@@ -5387,7 +5387,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
@@ -5395,7 +5395,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
@@ -5403,7 +5403,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -5411,7 +5411,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
@@ -5419,7 +5419,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13">
@@ -5427,7 +5427,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14">
@@ -5435,7 +5435,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
@@ -5443,7 +5443,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16">
@@ -5451,7 +5451,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -5459,7 +5459,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18">
@@ -5467,7 +5467,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
@@ -5475,7 +5475,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20">
@@ -5483,7 +5483,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21">
@@ -5491,7 +5491,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22">
@@ -5499,7 +5499,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23">
@@ -5507,7 +5507,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24">
@@ -5515,7 +5515,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25">
@@ -5523,7 +5523,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26">
@@ -5531,7 +5531,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27">
@@ -5539,7 +5539,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28">
@@ -5547,7 +5547,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29">
@@ -5571,7 +5571,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32">
@@ -5587,7 +5587,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34">
@@ -5595,7 +5595,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35">
@@ -5603,7 +5603,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36">
@@ -5611,7 +5611,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37">
@@ -5619,7 +5619,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38">
@@ -5627,7 +5627,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39">
@@ -5692,7 +5692,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
@@ -5700,7 +5700,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -5708,7 +5708,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -5716,7 +5716,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
@@ -5724,7 +5724,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
@@ -5732,7 +5732,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
@@ -5740,7 +5740,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
@@ -5748,7 +5748,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10">
@@ -5756,7 +5756,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11">
@@ -5764,7 +5764,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
@@ -5772,7 +5772,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
@@ -5780,7 +5780,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
@@ -5788,7 +5788,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15">
@@ -5796,7 +5796,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
@@ -5804,7 +5804,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -5812,7 +5812,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -5820,7 +5820,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19">
@@ -5828,7 +5828,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20">
@@ -5836,7 +5836,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21">
@@ -5844,7 +5844,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22">
@@ -5852,7 +5852,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23">
@@ -5860,7 +5860,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24">
@@ -5868,7 +5868,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25">
@@ -5876,7 +5876,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26">
@@ -5884,7 +5884,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27">
@@ -5892,7 +5892,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28">
@@ -5900,7 +5900,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29">
@@ -5924,7 +5924,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32">
@@ -5932,7 +5932,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33">
@@ -5940,7 +5940,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34">
@@ -5948,7 +5948,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35">
@@ -5964,7 +5964,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37">
@@ -5972,7 +5972,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38">
@@ -5980,7 +5980,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39">
@@ -6045,7 +6045,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
@@ -6053,7 +6053,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -6061,7 +6061,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -6069,7 +6069,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
@@ -6077,7 +6077,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
@@ -6085,7 +6085,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8">
@@ -6093,7 +6093,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
@@ -6101,7 +6101,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
@@ -6109,7 +6109,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11">
@@ -6117,7 +6117,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12">
@@ -6125,7 +6125,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
@@ -6133,7 +6133,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
@@ -6141,7 +6141,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15">
@@ -6149,7 +6149,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
@@ -6157,7 +6157,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17">
@@ -6165,7 +6165,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18">
@@ -6173,7 +6173,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19">
@@ -6181,7 +6181,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20">
@@ -6189,7 +6189,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21">
@@ -6197,7 +6197,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22">
@@ -6205,7 +6205,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23">
@@ -6213,7 +6213,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24">
@@ -6221,7 +6221,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25">
@@ -6229,7 +6229,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26">
@@ -6237,7 +6237,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27">
@@ -6245,7 +6245,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28">
@@ -6253,7 +6253,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29">
@@ -6269,7 +6269,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31">
@@ -6285,7 +6285,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33">
@@ -6293,7 +6293,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34">
@@ -6301,7 +6301,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35">
@@ -6309,7 +6309,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36">
@@ -6317,7 +6317,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37">
@@ -6325,7 +6325,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38">
@@ -6398,7 +6398,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
@@ -6422,7 +6422,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6">
@@ -6446,7 +6446,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9">
@@ -6454,7 +6454,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10">
@@ -6462,7 +6462,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
@@ -6470,7 +6470,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12">
@@ -6478,7 +6478,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13">
@@ -6486,7 +6486,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14">
@@ -6494,7 +6494,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15">
@@ -6502,7 +6502,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16">
@@ -6510,7 +6510,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17">
@@ -6518,7 +6518,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18">
@@ -6526,7 +6526,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19">
@@ -6534,7 +6534,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
@@ -6542,7 +6542,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21">
@@ -6550,7 +6550,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22">
@@ -6558,7 +6558,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23">
@@ -6566,7 +6566,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24">
@@ -6574,7 +6574,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25">
@@ -6582,7 +6582,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26">
@@ -6590,7 +6590,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27">
@@ -6598,7 +6598,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28">
@@ -6606,7 +6606,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29">
@@ -6751,7 +6751,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
@@ -6759,7 +6759,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4">
@@ -6791,7 +6791,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8">
@@ -6823,7 +6823,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12">
@@ -6831,7 +6831,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13">
@@ -6839,7 +6839,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14">
@@ -6847,7 +6847,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15">
@@ -6855,7 +6855,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16">
@@ -6863,7 +6863,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
@@ -6879,7 +6879,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19">
@@ -6887,7 +6887,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20">
@@ -6895,7 +6895,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21">
@@ -6903,7 +6903,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22">
@@ -6911,7 +6911,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23">
@@ -6919,7 +6919,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24">
@@ -6927,7 +6927,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25">
@@ -6935,7 +6935,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26">
@@ -6943,7 +6943,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27">
@@ -6951,7 +6951,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28">
@@ -6959,7 +6959,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29">
@@ -6967,7 +6967,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30">
@@ -7104,7 +7104,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3">
@@ -7112,7 +7112,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
@@ -7120,7 +7120,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
@@ -7160,7 +7160,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10">
@@ -7216,7 +7216,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17">
@@ -7224,7 +7224,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18">
@@ -7232,7 +7232,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19">
@@ -7240,7 +7240,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20">
@@ -7248,7 +7248,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21">
@@ -7256,7 +7256,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
@@ -7264,7 +7264,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23">
@@ -7288,7 +7288,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26">
@@ -7296,7 +7296,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27">
@@ -7304,7 +7304,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
@@ -7312,7 +7312,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29">
@@ -7320,7 +7320,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30">
@@ -7328,7 +7328,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31">
@@ -7336,7 +7336,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32">
@@ -7457,7 +7457,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -7465,7 +7465,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4">
@@ -7473,7 +7473,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
@@ -7529,7 +7529,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12">
@@ -7537,7 +7537,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13">
@@ -7545,7 +7545,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14">
@@ -7625,7 +7625,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24">
@@ -7633,7 +7633,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25">
@@ -7641,7 +7641,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26">
@@ -7649,7 +7649,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27">
@@ -7657,7 +7657,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28">
@@ -7665,7 +7665,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29">
@@ -7673,7 +7673,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30">
@@ -7681,7 +7681,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31">
@@ -7689,7 +7689,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32">
@@ -7697,7 +7697,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33">
@@ -7810,7 +7810,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3">
@@ -7818,7 +7818,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
@@ -7826,7 +7826,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
@@ -7834,7 +7834,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
@@ -7842,7 +7842,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
@@ -7850,7 +7850,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8">
@@ -7882,7 +7882,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12">
@@ -7890,7 +7890,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
@@ -7898,7 +7898,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14">
@@ -7906,7 +7906,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15">
@@ -7914,7 +7914,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16">
@@ -7922,7 +7922,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17">
@@ -8010,7 +8010,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28">
@@ -8018,7 +8018,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29">
@@ -8026,7 +8026,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
@@ -8034,7 +8034,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31">
@@ -8042,7 +8042,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32">
@@ -8050,7 +8050,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33">
@@ -8058,7 +8058,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34">
@@ -8163,7 +8163,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
@@ -8171,7 +8171,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
@@ -8179,7 +8179,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
@@ -8187,7 +8187,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
@@ -8195,7 +8195,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
@@ -8379,7 +8379,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30">
@@ -8387,7 +8387,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31">
@@ -8395,7 +8395,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32">
@@ -8403,7 +8403,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33">
@@ -8411,7 +8411,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34">
@@ -8419,7 +8419,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35">
@@ -8516,7 +8516,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3">
@@ -8524,7 +8524,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
@@ -8740,7 +8740,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31">
@@ -8748,7 +8748,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32">
@@ -8756,7 +8756,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33">
@@ -8764,7 +8764,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34">
@@ -8772,7 +8772,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35">
@@ -8780,7 +8780,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36">

</xml_diff>